<commit_message>
Reorganised folders and added documentation folder from google drive
</commit_message>
<xml_diff>
--- a/Payslip process/DataBases/payslip_template_employees.xlsx
+++ b/Payslip process/DataBases/payslip_template_employees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Payslip process\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0C6AD0-4F14-444C-8E7F-ABE20844748D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF01A55-5712-4680-8D77-C1D418872C25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25440" yWindow="5175" windowWidth="14400" windowHeight="10755" xr2:uid="{F02BCD34-8A2E-4C13-922F-FC2A6D996D89}"/>
+    <workbookView xWindow="21285" yWindow="6660" windowWidth="21240" windowHeight="8550" xr2:uid="{F02BCD34-8A2E-4C13-922F-FC2A6D996D89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -820,13 +820,13 @@
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="11">
-        <v>640</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
         <v>14</v>
       </c>
       <c r="I11" s="12">
-        <v>640</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>